<commit_message>
Ok Log Map Cargo, pendiente pruebas
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\FinalizacionLocalizacionMercancias_2.0.4\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\FinalizacionLocalizacionMercancias_2.0.5\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890C8F17-DB58-4605-8F46-9CBE32EC5424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0DB33A-86F0-4AFB-8D12-6A306018FE8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -981,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Avance consulta DO Muisca por URL dinamica
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\FinalizacionLocalizacionMercancias_2.0.5\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\FinalizacionLocalizacionMercancias_2.0.9\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0DB33A-86F0-4AFB-8D12-6A306018FE8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E3A824-12AD-40B8-A2B4-ED61106134E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -75,22 +75,10 @@
     <t>Error de Autenticacion</t>
   </si>
   <si>
-    <t>URL_Importaciones</t>
-  </si>
-  <si>
-    <t>https://importaciones.dian.gov.co/</t>
-  </si>
-  <si>
     <t>ConexionBD</t>
   </si>
   <si>
     <t>Dsn=RPA</t>
-  </si>
-  <si>
-    <t>select * from dwf_content.rpa_procesos where pro_lote = '{0}' and estado = '{1}' limit {2};</t>
-  </si>
-  <si>
-    <t>update dwf_content.rpa_procesos set estado = '{0}' where pro_id = '{1}'</t>
   </si>
   <si>
     <t>MaxRetryNumber</t>
@@ -231,19 +219,10 @@
     <t>Mensaje de error de autenticación</t>
   </si>
   <si>
-    <t>URL principal para la automatización</t>
-  </si>
-  <si>
     <t>MSG_ERRORDOCUMENTOSSOPORTE</t>
   </si>
   <si>
     <t>Se presentaron Errores al Radicar Documentos</t>
-  </si>
-  <si>
-    <t>QueryAceptacionRegLote</t>
-  </si>
-  <si>
-    <t>QueryAceptacionUpdateEstado</t>
   </si>
   <si>
     <t>true</t>
@@ -600,6 +579,51 @@
   <si>
     <t>El Documento {0} no tiene manifiesto en consulta de documentos. No existe en Muisca por documentos declarantes</t>
   </si>
+  <si>
+    <t>URL_MuiscaDocumentos</t>
+  </si>
+  <si>
+    <t>URL_MuiscaDocumentosDeclarantes</t>
+  </si>
+  <si>
+    <t>URL_MuiscaDocumentosPerfilados</t>
+  </si>
+  <si>
+    <t>URL_MuiscaMigradosSYGA</t>
+  </si>
+  <si>
+    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteConsDocumentos&amp;PU_ide_administracion={0}&amp; PU_val_doc_transporte={1}&amp;  PU_tipo_doc_transporte=10910097&amp;PU_num_ident_transportador=830004237&amp;PR_datasource=importacion.reportes.DCmdSrvConsManifiestoDocTransporte</t>
+  </si>
+  <si>
+    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteDocAgenteAduana&amp;PU_ide_administracion={0}&amp;PU_val_doc_transporte={1}&amp;PR_datasource=MuiscaDS</t>
+  </si>
+  <si>
+    <t>Consulta documentos declarantes de Muisca por URL dinamica con Id Administración y Documento de transporte como parametros de entrada</t>
+  </si>
+  <si>
+    <t>Consulta documentos de Muisca por URL dinamica con Id Administración y Documento de transporte como parametros de entrada</t>
+  </si>
+  <si>
+    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteInclusion&amp;PU_ide_administracion={0}&amp;PU_val_num_doc_transp={1}&amp;PR_datasource=MuiscaDS</t>
+  </si>
+  <si>
+    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteTranSyga&amp;PU_ide_manifiesto={0}&amp; PU_guia={1}&amp; PR_datasource=MuiscaDS</t>
+  </si>
+  <si>
+    <t>Consulta documentos perfilados de Muisca por URL dinamica con Id Administración y Documento de transporte como parametros de entrada</t>
+  </si>
+  <si>
+    <t>Consulta documentos migrados a SYGA de Muisca por URL dinamica con Manifiesto y Documento de transporte como parametros de entrada</t>
+  </si>
+  <si>
+    <t>INSERT INTO RPA.rpa_suc (SUCIDXXX, SUCDESXX, SUCCODXX, REGUSRXX, REGFECXX, REGHORXX, REGUSRMX, REGFECMX, REGHORMX, REGESTXX, REGSTAMP) VALUES ('{0}', '{1}', '{2}', '{3}', '{4}', '{5}', '', '', '', '', CURRENT_TIMESTAMP);</t>
+  </si>
+  <si>
+    <t>QueryRegSucursalNueva</t>
+  </si>
+  <si>
+    <t>User_ConexionGRM</t>
+  </si>
 </sst>
 </file>
 
@@ -654,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -665,6 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1057,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1066,7 +1091,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -1097,7 +1122,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -1162,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -1196,7 +1221,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -1230,7 +1255,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
@@ -1264,7 +1289,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -1298,7 +1323,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -1326,10 +1351,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -1358,10 +1383,10 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -1390,10 +1415,10 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -1422,10 +1447,10 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -1454,10 +1479,10 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -1486,10 +1511,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -1518,10 +1543,10 @@
     </row>
     <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -1550,10 +1575,10 @@
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C18"/>
       <c r="D18"/>
@@ -1582,10 +1607,10 @@
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -1614,10 +1639,10 @@
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -1646,10 +1671,10 @@
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -1678,10 +1703,10 @@
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C22"/>
       <c r="D22"/>
@@ -1710,10 +1735,10 @@
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -1742,10 +1767,10 @@
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C24"/>
       <c r="D24"/>
@@ -1774,10 +1799,10 @@
     </row>
     <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -1806,10 +1831,10 @@
     </row>
     <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -1838,10 +1863,10 @@
     </row>
     <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
@@ -1870,10 +1895,10 @@
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
@@ -1902,10 +1927,10 @@
     </row>
     <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
@@ -1934,10 +1959,10 @@
     </row>
     <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -1966,10 +1991,10 @@
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -1998,10 +2023,10 @@
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -2030,10 +2055,10 @@
     </row>
     <row r="33" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -2062,10 +2087,10 @@
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
@@ -2094,10 +2119,10 @@
     </row>
     <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C35"/>
       <c r="D35"/>
@@ -2126,10 +2151,10 @@
     </row>
     <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C36"/>
       <c r="D36"/>
@@ -2158,10 +2183,10 @@
     </row>
     <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C37"/>
       <c r="D37"/>
@@ -2218,10 +2243,10 @@
     </row>
     <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C39"/>
       <c r="D39"/>
@@ -2250,10 +2275,10 @@
     </row>
     <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C40"/>
       <c r="D40"/>
@@ -2282,13 +2307,13 @@
     </row>
     <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D41"/>
       <c r="E41"/>
@@ -2316,13 +2341,13 @@
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D42"/>
       <c r="E42"/>
@@ -2350,10 +2375,10 @@
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C43"/>
       <c r="D43"/>
@@ -2381,9 +2406,15 @@
       <c r="Z43"/>
     </row>
     <row r="44" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
+      <c r="A44" t="s">
+        <v>185</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" t="s">
+        <v>192</v>
+      </c>
       <c r="D44"/>
       <c r="E44"/>
       <c r="F44"/>
@@ -2409,14 +2440,14 @@
       <c r="Z44"/>
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>17</v>
+      <c r="A45" t="s">
+        <v>186</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>18</v>
+      <c r="B45" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="D45"/>
       <c r="E45"/>
@@ -2443,9 +2474,15 @@
       <c r="Z45"/>
     </row>
     <row r="46" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
+      <c r="A46" t="s">
+        <v>187</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" t="s">
+        <v>195</v>
+      </c>
       <c r="D46"/>
       <c r="E46"/>
       <c r="F46"/>
@@ -2471,14 +2508,14 @@
       <c r="Z46"/>
     </row>
     <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>19</v>
+      <c r="A47" t="s">
+        <v>188</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>75</v>
+      <c r="B47" s="3" t="s">
+        <v>194</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>20</v>
+      <c r="C47" t="s">
+        <v>196</v>
       </c>
       <c r="D47"/>
       <c r="E47"/>
@@ -2505,12 +2542,8 @@
       <c r="Z47"/>
     </row>
     <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="A48"/>
+      <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
@@ -2538,12 +2571,14 @@
     </row>
     <row r="49" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>77</v>
+      <c r="B49" s="1" t="s">
+        <v>68</v>
       </c>
-      <c r="C49"/>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D49"/>
       <c r="E49"/>
       <c r="F49"/>
@@ -2570,10 +2605,10 @@
     </row>
     <row r="50" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>79</v>
+      <c r="B50" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C50"/>
       <c r="D50"/>
@@ -2600,12 +2635,12 @@
       <c r="Y50"/>
       <c r="Z50"/>
     </row>
-    <row r="51" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="C51"/>
       <c r="D51"/>
@@ -2633,6 +2668,12 @@
       <c r="Z51"/>
     </row>
     <row r="52" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
@@ -2658,12 +2699,12 @@
       <c r="Y52"/>
       <c r="Z52"/>
     </row>
-    <row r="53" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>72</v>
+    <row r="53" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>141</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>21</v>
+      <c r="B53" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="C53"/>
       <c r="D53"/>
@@ -2690,12 +2731,12 @@
       <c r="Y53"/>
       <c r="Z53"/>
     </row>
-    <row r="54" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>73</v>
+    <row r="54" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>198</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>22</v>
+      <c r="B54" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="C54"/>
       <c r="D54"/>
@@ -2750,10 +2791,10 @@
     </row>
     <row r="56" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C56"/>
       <c r="D56"/>
@@ -2782,10 +2823,10 @@
     </row>
     <row r="57" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C57"/>
       <c r="D57"/>
@@ -2814,10 +2855,10 @@
     </row>
     <row r="58" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C58"/>
       <c r="D58"/>
@@ -2846,10 +2887,10 @@
     </row>
     <row r="59" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C59"/>
       <c r="D59"/>
@@ -2878,10 +2919,10 @@
     </row>
     <row r="60" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C60"/>
       <c r="D60"/>
@@ -2910,10 +2951,10 @@
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C61"/>
       <c r="D61"/>
@@ -2942,10 +2983,10 @@
     </row>
     <row r="62" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C62"/>
       <c r="D62"/>
@@ -2974,10 +3015,10 @@
     </row>
     <row r="63" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C63"/>
       <c r="D63"/>
@@ -3006,10 +3047,10 @@
     </row>
     <row r="64" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C64"/>
       <c r="D64"/>
@@ -3038,10 +3079,10 @@
     </row>
     <row r="65" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C65"/>
       <c r="D65"/>
@@ -3098,7 +3139,7 @@
     </row>
     <row r="67" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B67">
         <v>100</v>
@@ -3158,10 +3199,10 @@
     </row>
     <row r="69" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C69"/>
       <c r="D69"/>
@@ -3190,10 +3231,10 @@
     </row>
     <row r="70" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C70"/>
       <c r="D70"/>
@@ -3222,10 +3263,10 @@
     </row>
     <row r="71" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C71"/>
       <c r="D71"/>
@@ -3254,10 +3295,10 @@
     </row>
     <row r="72" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C72"/>
       <c r="D72"/>
@@ -3286,10 +3327,10 @@
     </row>
     <row r="73" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B73" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C73"/>
       <c r="D73"/>
@@ -3318,10 +3359,10 @@
     </row>
     <row r="74" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C74"/>
       <c r="D74"/>
@@ -3350,10 +3391,10 @@
     </row>
     <row r="75" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C75"/>
       <c r="D75"/>
@@ -3382,10 +3423,10 @@
     </row>
     <row r="76" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C76"/>
       <c r="D76"/>
@@ -3414,10 +3455,10 @@
     </row>
     <row r="77" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C77"/>
       <c r="D77"/>
@@ -3446,10 +3487,10 @@
     </row>
     <row r="78" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
@@ -3478,10 +3519,10 @@
     </row>
     <row r="79" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C79"/>
       <c r="D79"/>
@@ -3510,10 +3551,10 @@
     </row>
     <row r="80" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C80"/>
       <c r="D80"/>
@@ -3569,8 +3610,12 @@
       <c r="Z81"/>
     </row>
     <row r="82" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
+      <c r="A82" t="s">
+        <v>199</v>
+      </c>
+      <c r="B82" s="8">
+        <v>12345678910</v>
+      </c>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82"/>
@@ -30171,13 +30216,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -30205,7 +30250,7 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -30265,13 +30310,13 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>5000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -30299,13 +30344,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>30000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -30333,13 +30378,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1">
         <v>120000</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
@@ -30395,13 +30440,13 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -30457,13 +30502,13 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1">
         <v>1000</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -30491,13 +30536,13 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1">
         <v>15000</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -30525,13 +30570,13 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1">
         <v>60000</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -30587,13 +30632,13 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>0.6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -30621,13 +30666,13 @@
     </row>
     <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1">
         <v>0.8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -30655,13 +30700,13 @@
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1">
         <v>0.9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -30717,13 +30762,13 @@
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
@@ -30751,13 +30796,13 @@
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D21"/>
       <c r="E21"/>
@@ -30785,13 +30830,13 @@
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
@@ -30819,13 +30864,13 @@
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D23"/>
       <c r="E23"/>
@@ -30853,13 +30898,13 @@
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D24"/>
       <c r="E24"/>
@@ -58262,10 +58307,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>

</xml_diff>

<commit_message>
Avance2 consulta DO Muisca por URL dinamica
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\FinalizacionLocalizacionMercancias_2.0.9\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E3A824-12AD-40B8-A2B4-ED61106134E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9C2F9D-AF17-4577-9449-873637C0EF44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Consulta por Link en todo Muisca
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\FinalizacionLocalizacionMercancias_2.0.9\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9C2F9D-AF17-4577-9449-873637C0EF44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0882D56C-A90A-415E-9BB7-ABA62D4C1E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="202">
   <si>
     <t>Name</t>
   </si>
@@ -592,9 +592,6 @@
     <t>URL_MuiscaMigradosSYGA</t>
   </si>
   <si>
-    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteConsDocumentos&amp;PU_ide_administracion={0}&amp; PU_val_doc_transporte={1}&amp;  PU_tipo_doc_transporte=10910097&amp;PU_num_ident_transportador=830004237&amp;PR_datasource=importacion.reportes.DCmdSrvConsManifiestoDocTransporte</t>
-  </si>
-  <si>
     <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteDocAgenteAduana&amp;PU_ide_administracion={0}&amp;PU_val_doc_transporte={1}&amp;PR_datasource=MuiscaDS</t>
   </si>
   <si>
@@ -605,9 +602,6 @@
   </si>
   <si>
     <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteInclusion&amp;PU_ide_administracion={0}&amp;PU_val_num_doc_transp={1}&amp;PR_datasource=MuiscaDS</t>
-  </si>
-  <si>
-    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteTranSyga&amp;PU_ide_manifiesto={0}&amp; PU_guia={1}&amp; PR_datasource=MuiscaDS</t>
   </si>
   <si>
     <t>Consulta documentos perfilados de Muisca por URL dinamica con Id Administración y Documento de transporte como parametros de entrada</t>
@@ -623,6 +617,18 @@
   </si>
   <si>
     <t>User_ConexionGRM</t>
+  </si>
+  <si>
+    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteConsDocumentos&amp;PU_ide_administracion={0}&amp;PU_val_doc_transporte={1}&amp;PU_tipo_doc_transporte=10910097&amp;PU_num_ident_transportador=830004237&amp;PR_datasource=importacion.reportes.DCmdSrvConsManifiestoDocTransporte</t>
+  </si>
+  <si>
+    <t>https://importacionescarga.dian.gov.co/WebImportacion/DefMostrarReporteVacio.faces?PR_reporte=reporteTranSyga&amp;PU_ide_manifiesto={0}&amp;PU_guia={1}&amp;PR_datasource=MuiscaDS</t>
+  </si>
+  <si>
+    <t>MSG_ERROR_NOMATCH_MUISCA</t>
+  </si>
+  <si>
+    <t>Documento: {0} No concuerda con Consignatario y Fecha Aviso Llegada</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1028"/>
+  <dimension ref="A1:Z1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1991,10 +1997,10 @@
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="C31"/>
       <c r="D31"/>
@@ -2023,10 +2029,10 @@
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C32"/>
       <c r="D32"/>
@@ -2055,10 +2061,10 @@
     </row>
     <row r="33" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
@@ -2087,10 +2093,10 @@
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
@@ -2119,10 +2125,10 @@
     </row>
     <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C35"/>
       <c r="D35"/>
@@ -2151,10 +2157,10 @@
     </row>
     <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C36"/>
       <c r="D36"/>
@@ -2183,10 +2189,10 @@
     </row>
     <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C37"/>
       <c r="D37"/>
@@ -2214,8 +2220,12 @@
       <c r="Z37"/>
     </row>
     <row r="38" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
+      <c r="A38" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
@@ -2242,12 +2252,8 @@
       <c r="Z38"/>
     </row>
     <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="A39"/>
+      <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
@@ -2275,10 +2281,10 @@
     </row>
     <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>74</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="C40"/>
       <c r="D40"/>
@@ -2307,14 +2313,12 @@
     </row>
     <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
-      <c r="C41" t="s">
-        <v>156</v>
-      </c>
+      <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
@@ -2341,13 +2345,13 @@
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D42"/>
       <c r="E42"/>
@@ -2375,12 +2379,14 @@
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
-      <c r="C43"/>
+      <c r="C43" t="s">
+        <v>157</v>
+      </c>
       <c r="D43"/>
       <c r="E43"/>
       <c r="F43"/>
@@ -2407,14 +2413,12 @@
     </row>
     <row r="44" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
-      <c r="C44" t="s">
-        <v>192</v>
-      </c>
+      <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
       <c r="F44"/>
@@ -2441,10 +2445,10 @@
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C45" t="s">
         <v>191</v>
@@ -2475,13 +2479,13 @@
     </row>
     <row r="46" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D46"/>
       <c r="E46"/>
@@ -2509,13 +2513,13 @@
     </row>
     <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C47" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D47"/>
       <c r="E47"/>
@@ -2542,9 +2546,15 @@
       <c r="Z47"/>
     </row>
     <row r="48" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
+      <c r="A48" t="s">
+        <v>188</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" t="s">
+        <v>194</v>
+      </c>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
@@ -2570,15 +2580,9 @@
       <c r="Z48"/>
     </row>
     <row r="49" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
       <c r="D49"/>
       <c r="E49"/>
       <c r="F49"/>
@@ -2605,12 +2609,14 @@
     </row>
     <row r="50" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
-      <c r="C50"/>
+      <c r="C50" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D50"/>
       <c r="E50"/>
       <c r="F50"/>
@@ -2637,10 +2643,10 @@
     </row>
     <row r="51" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>70</v>
+      <c r="B51" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C51"/>
       <c r="D51"/>
@@ -2669,10 +2675,10 @@
     </row>
     <row r="52" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C52"/>
       <c r="D52"/>
@@ -2699,12 +2705,12 @@
       <c r="Y52"/>
       <c r="Z52"/>
     </row>
-    <row r="53" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="C53"/>
       <c r="D53"/>
@@ -2733,10 +2739,10 @@
     </row>
     <row r="54" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>197</v>
+        <v>143</v>
       </c>
       <c r="C54"/>
       <c r="D54"/>
@@ -2763,7 +2769,13 @@
       <c r="Y54"/>
       <c r="Z54"/>
     </row>
-    <row r="55" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="C55"/>
       <c r="D55"/>
       <c r="E55"/>
@@ -2790,12 +2802,6 @@
       <c r="Z55"/>
     </row>
     <row r="56" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="C56"/>
       <c r="D56"/>
       <c r="E56"/>
@@ -2823,10 +2829,10 @@
     </row>
     <row r="57" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C57"/>
       <c r="D57"/>
@@ -2855,10 +2861,10 @@
     </row>
     <row r="58" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C58"/>
       <c r="D58"/>
@@ -2886,11 +2892,11 @@
       <c r="Z58"/>
     </row>
     <row r="59" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>149</v>
+      <c r="A59" s="1" t="s">
+        <v>90</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>126</v>
+      <c r="B59" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="C59"/>
       <c r="D59"/>
@@ -2919,10 +2925,10 @@
     </row>
     <row r="60" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>82</v>
+      <c r="B60" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="C60"/>
       <c r="D60"/>
@@ -2951,10 +2957,10 @@
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="C61"/>
       <c r="D61"/>
@@ -2983,10 +2989,10 @@
     </row>
     <row r="62" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="C62"/>
       <c r="D62"/>
@@ -3015,10 +3021,10 @@
     </row>
     <row r="63" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="C63"/>
       <c r="D63"/>
@@ -3047,10 +3053,10 @@
     </row>
     <row r="64" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>83</v>
+      <c r="B64" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C64"/>
       <c r="D64"/>
@@ -3079,7 +3085,7 @@
     </row>
     <row r="65" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>83</v>
@@ -3110,8 +3116,12 @@
       <c r="Z65"/>
     </row>
     <row r="66" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66"/>
-      <c r="B66"/>
+      <c r="A66" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66"/>
@@ -3138,12 +3148,8 @@
       <c r="Z66"/>
     </row>
     <row r="67" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67">
-        <v>100</v>
-      </c>
+      <c r="A67"/>
+      <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
       <c r="E67"/>
@@ -3170,8 +3176,12 @@
       <c r="Z67"/>
     </row>
     <row r="68" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
+      <c r="A68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68">
+        <v>100</v>
+      </c>
       <c r="C68"/>
       <c r="D68"/>
       <c r="E68"/>
@@ -3198,12 +3208,8 @@
       <c r="Z68"/>
     </row>
     <row r="69" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" t="s">
-        <v>104</v>
-      </c>
+      <c r="A69"/>
+      <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
       <c r="E69"/>
@@ -3231,10 +3237,10 @@
     </row>
     <row r="70" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C70"/>
       <c r="D70"/>
@@ -3263,10 +3269,10 @@
     </row>
     <row r="71" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C71"/>
       <c r="D71"/>
@@ -3295,10 +3301,10 @@
     </row>
     <row r="72" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C72"/>
       <c r="D72"/>
@@ -3327,10 +3333,10 @@
     </row>
     <row r="73" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C73"/>
       <c r="D73"/>
@@ -3359,10 +3365,10 @@
     </row>
     <row r="74" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C74"/>
       <c r="D74"/>
@@ -3391,10 +3397,10 @@
     </row>
     <row r="75" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C75"/>
       <c r="D75"/>
@@ -3423,10 +3429,10 @@
     </row>
     <row r="76" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C76"/>
       <c r="D76"/>
@@ -3455,10 +3461,10 @@
     </row>
     <row r="77" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C77"/>
       <c r="D77"/>
@@ -3487,10 +3493,10 @@
     </row>
     <row r="78" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
@@ -3519,10 +3525,10 @@
     </row>
     <row r="79" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C79"/>
       <c r="D79"/>
@@ -3551,10 +3557,10 @@
     </row>
     <row r="80" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B80" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C80"/>
       <c r="D80"/>
@@ -3582,8 +3588,12 @@
       <c r="Z80"/>
     </row>
     <row r="81" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81"/>
-      <c r="B81"/>
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" t="s">
+        <v>115</v>
+      </c>
       <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
@@ -3610,12 +3620,8 @@
       <c r="Z81"/>
     </row>
     <row r="82" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>199</v>
-      </c>
-      <c r="B82" s="8">
-        <v>12345678910</v>
-      </c>
+      <c r="A82"/>
+      <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82"/>
@@ -3642,8 +3648,12 @@
       <c r="Z82"/>
     </row>
     <row r="83" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
+      <c r="A83" t="s">
+        <v>197</v>
+      </c>
+      <c r="B83" s="8">
+        <v>12345678910</v>
+      </c>
       <c r="C83"/>
       <c r="D83"/>
       <c r="E83"/>
@@ -30128,6 +30138,34 @@
       <c r="X1028"/>
       <c r="Y1028"/>
       <c r="Z1028"/>
+    </row>
+    <row r="1029" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1029"/>
+      <c r="B1029"/>
+      <c r="C1029"/>
+      <c r="D1029"/>
+      <c r="E1029"/>
+      <c r="F1029"/>
+      <c r="G1029"/>
+      <c r="H1029"/>
+      <c r="I1029"/>
+      <c r="J1029"/>
+      <c r="K1029"/>
+      <c r="L1029"/>
+      <c r="M1029"/>
+      <c r="N1029"/>
+      <c r="O1029"/>
+      <c r="P1029"/>
+      <c r="Q1029"/>
+      <c r="R1029"/>
+      <c r="S1029"/>
+      <c r="T1029"/>
+      <c r="U1029"/>
+      <c r="V1029"/>
+      <c r="W1029"/>
+      <c r="X1029"/>
+      <c r="Y1029"/>
+      <c r="Z1029"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>